<commit_message>
Update Problem Set 3_AllenWalker.xlsx
</commit_message>
<xml_diff>
--- a/Problem Set 3_AllenWalker.xlsx
+++ b/Problem Set 3_AllenWalker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53a11ba7f4d0debc/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="508" documentId="8_{0AF5A2A4-7C82-7E4F-A6DE-7D3B53A26F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1D914D8-9348-2043-A3F3-6934A2C7EC28}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1C4F7DF-BC1B-4D43-8ACF-D65FF4A59DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15540" yWindow="2160" windowWidth="12660" windowHeight="14180" activeTab="6" xr2:uid="{740FD8DC-7B53-4E78-8E3A-26D1AA96C0C6}"/>
+    <workbookView xWindow="37200" yWindow="2220" windowWidth="26240" windowHeight="14180" activeTab="6" xr2:uid="{740FD8DC-7B53-4E78-8E3A-26D1AA96C0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1" sheetId="2" r:id="rId1"/>
@@ -24,26 +24,24 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Question 2'!$A$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Question 2'!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Question 2'!$C$1:$C$7</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Question 2'!$C$8:$C$41</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Question 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Question 2'!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Question 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Question 2'!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'Question 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'Question 2'!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Question 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Question 2'!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Question 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Question 2'!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Question 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Question 2'!$A$2:$A$41</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Question 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Question 2'!$A$2:$A$41</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Question 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Question 2'!$D$2:$D$7</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Question 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Question 2'!$E$2:$E$7</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'Question 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'Question 2'!$F$2:$F$7</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Question 2'!$C$2:$C$7</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Question 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Question 2'!$D$2:$D$7</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Question 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Question 2'!$E$2:$E$7</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Question 2'!$F$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Question 2'!$F$2:$F$7</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Question 2'!$C$2:$C$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="24" r:id="rId8"/>
+    <pivotCache cacheId="27" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -279,7 +277,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -387,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -411,26 +409,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -935,8 +932,27 @@
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
       <cx:numDim type="val">
+        <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:strDim type="cat">
         <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -971,17 +987,58 @@
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{DAC1B4F6-3B12-044D-BDA2-A322358FC0F7}">
+        <cx:series layoutId="clusteredColumn" uniqueId="{C9FE10B7-E1E3-A94F-9CF6-4F7B58F1D555}" formatIdx="0">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
-              <cx:v>Data</cx:v>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>Frequency Distribution</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
           <cx:layoutPr>
-            <cx:binning intervalClosed="r"/>
+            <cx:aggregation/>
           </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{EA6DCC49-9CFF-7340-8EEF-0662E60BA4D4}" formatIdx="1">
+          <cx:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </cx:spPr>
+          <cx:axisId val="2"/>
+        </cx:series>
+        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{55CFCD17-659B-7647-A94A-511C5B7E06BE}" formatIdx="2">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:v>Relative Frequency</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:aggregation/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="2" uniqueId="{927CD6CD-2755-D84A-BB38-54DD973C1773}" formatIdx="3">
+          <cx:axisId val="2"/>
+        </cx:series>
+        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{0E2FF8C5-D07B-A348-8A91-C6D3342A5621}" formatIdx="4">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>Percent Frequency</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:aggregation/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="4" uniqueId="{8E1E1CD9-CDBA-3D4A-9416-2F2C5CBA2889}" formatIdx="5">
+          <cx:axisId val="2"/>
         </cx:series>
       </cx:plotAreaRegion>
       <cx:axis id="0">
@@ -991,6 +1048,11 @@
       <cx:axis id="1">
         <cx:valScaling/>
         <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
@@ -2475,24 +2537,24 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="Chart 3">
+            <xdr:cNvPr id="3" name="Chart 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D474A82-2891-9477-7969-4E000E2F77CC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64E03EA8-3F42-F93A-924E-701AD7AF07DA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2519,7 +2581,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2698750" y="2749550"/>
+              <a:off x="2781300" y="2882900"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3772,7 +3834,7 @@
     <worksheetSource ref="B1:B21" sheet="Question 5"/>
   </cacheSource>
   <cacheFields count="1">
-    <cacheField name="# U.S. Locations" numFmtId="165">
+    <cacheField name="# U.S. Locations" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1431" maxValue="37496" count="20">
         <n v="1864"/>
         <n v="3183"/>
@@ -3871,10 +3933,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{645468FC-3A0C-4F41-9A15-3DCDA0CDA764}" name="PivotTable6" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{645468FC-3A0C-4F41-9A15-3DCDA0CDA764}" name="PivotTable6" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="1">
-    <pivotField axis="axisCol" dataField="1" numFmtId="165" showAll="0">
+    <pivotField axis="axisCol" dataField="1" numFmtId="164" showAll="0">
       <items count="21">
         <item x="18"/>
         <item x="7"/>
@@ -4361,7 +4423,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4820,7 +4882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFE55A6-6D91-430E-953E-83F77C249245}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -4834,193 +4896,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="20">
         <v>325000.78000000003</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="19">
         <v>124</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>12499.3452</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="21">
         <f>B2/C2</f>
         <v>2620.9740322580647</v>
       </c>
-      <c r="F2" s="20"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>13678.21</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>9</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <v>239.9434</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <f t="shared" ref="E3:E10" si="0">B3/C3</f>
         <v>1519.8011111111109</v>
       </c>
-      <c r="F3" s="20"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>452359.19</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>175</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>21987.246200000001</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="21">
         <f t="shared" si="0"/>
         <v>2584.9096571428572</v>
       </c>
-      <c r="F4" s="20"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>87423.91</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>28</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>7642.9011</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <f t="shared" si="0"/>
         <v>3122.2825000000003</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>87654.21</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>21</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>1250.1393</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="21">
         <f t="shared" si="0"/>
         <v>4174.01</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>234091.39</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>48</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>14567.9833</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <f t="shared" si="0"/>
         <v>4876.9039583333333</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>379401.94</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>121</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>27981.443200000002</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <f t="shared" si="0"/>
         <v>3135.5532231404959</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>31733.59</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>7</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>672.91110000000003</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <f t="shared" si="0"/>
         <v>4533.37</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <v>127845.22</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <v>17</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>13322.971299999999</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <f t="shared" si="0"/>
         <v>7520.3070588235296</v>
       </c>
-      <c r="F10" s="20"/>
+      <c r="F10" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5221,7 +5283,7 @@
   <dimension ref="A3:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5237,72 +5299,72 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="18">
+      <c r="B4" s="17">
         <v>1431</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>1572</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>1618</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>1668</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>1864</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>1877</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <v>1901</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="17">
         <v>2130</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="17">
         <v>2155</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="17">
         <v>3183</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="17">
         <v>5018</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <v>7683</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="17">
         <v>9947</v>
       </c>
-      <c r="O4" s="18">
+      <c r="O4" s="17">
         <v>12394</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="17">
         <v>13281</v>
       </c>
-      <c r="Q4" s="18">
+      <c r="Q4" s="17">
         <v>16224</v>
       </c>
-      <c r="R4" s="18">
+      <c r="R4" s="17">
         <v>25199</v>
       </c>
-      <c r="S4" s="18">
+      <c r="S4" s="17">
         <v>32805</v>
       </c>
-      <c r="T4" s="18">
+      <c r="T4" s="17">
         <v>34871</v>
       </c>
-      <c r="U4" s="18">
+      <c r="U4" s="17">
         <v>37496</v>
       </c>
-      <c r="V4" s="18" t="s">
+      <c r="V4" s="17" t="s">
         <v>66</v>
       </c>
     </row>
@@ -5310,67 +5372,66 @@
       <c r="A5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5">
         <v>6</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5">
         <v>7</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5">
         <v>8</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5">
         <v>9</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5">
         <v>10</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5">
         <v>11</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5">
         <v>12</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5">
         <v>13</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5">
         <v>14</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5">
         <v>15</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5">
         <v>16</v>
       </c>
-      <c r="R5" s="16">
+      <c r="R5">
         <v>17</v>
       </c>
-      <c r="S5" s="16">
+      <c r="S5">
         <v>18</v>
       </c>
-      <c r="T5" s="16">
+      <c r="T5">
         <v>19</v>
       </c>
-      <c r="U5" s="16">
+      <c r="U5">
         <v>20</v>
       </c>
-      <c r="V5" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>